<commit_message>
About to change ExcelTemplate structure.  So I want the current version.
</commit_message>
<xml_diff>
--- a/Excel Import Transform - Dino.xlsx
+++ b/Excel Import Transform - Dino.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Projects\PLSO2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03850996-2F0A-4D10-910A-17B4510F993D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3691BCB-996A-4D48-A3CE-7DD70F17F667}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="9720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,7 +359,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -829,11 +829,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -846,7 +846,7 @@
     <col min="9" max="9" width="83.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -875,7 +875,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -889,7 +889,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -915,7 +915,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -935,7 +935,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -952,7 +952,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -978,7 +978,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1308,12 +1308,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>24</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>27</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>34</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
         <v>43</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>45</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>50</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>53</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
         <v>66</v>
       </c>
@@ -1483,10 +1483,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F32"/>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
         <v>59</v>
       </c>
@@ -1510,10 +1510,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F36" s="12" t="s">
         <v>92</v>
       </c>
@@ -1532,10 +1532,10 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -1544,7 +1544,7 @@
     <col min="6" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>108</v>
       </c>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>53</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>2</v>
       </c>
@@ -1718,7 +1718,7 @@
       <c r="E10" s="23"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>5</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>14</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>106</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>45</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>50</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>12</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>104</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>24</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>3</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>4</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>

</xml_diff>